<commit_message>
CSV Float load bug fix
</commit_message>
<xml_diff>
--- a/TableBuilder/xlsx_Data/PropertyTable.xlsx
+++ b/TableBuilder/xlsx_Data/PropertyTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="126">
   <si>
     <t>!EndOfTable</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -357,10 +357,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>wander_range</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>walkSpeed</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -373,10 +369,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>angular_speed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>attack_power</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -418,6 +410,94 @@
   </si>
   <si>
     <t>Player</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>wander_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>min_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>wander_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>max_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>range</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stoppingDist</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>angular</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>peed</t>
+    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -646,7 +726,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -685,12 +765,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="10" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="10" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1006,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1018,36 +1101,40 @@
     <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.19921875" customWidth="1"/>
+    <col min="5" max="5" width="17.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.19921875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14" t="s">
-        <v>119</v>
-      </c>
+      <c r="B1" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
       <c r="K1" s="14"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L1" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1060,34 +1147,40 @@
       <c r="D2" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="I2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>104</v>
@@ -1113,19 +1206,25 @@
       <c r="I3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="L3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1137,10 +1236,12 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1149,19 +1250,21 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="5">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5">
         <v>100</v>
       </c>
-      <c r="J5" s="5">
+      <c r="L5" s="5">
         <v>1</v>
       </c>
-      <c r="K5" s="5">
+      <c r="M5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" s="5">
         <v>15</v>
@@ -1173,30 +1276,36 @@
         <v>1.5</v>
       </c>
       <c r="E6" s="5">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F6" s="5">
+        <v>30</v>
+      </c>
+      <c r="G6" s="5">
         <v>1200</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="I6" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="5">
+        <v>2</v>
+      </c>
+      <c r="L6" s="5">
         <v>1</v>
       </c>
-      <c r="H6" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="I6" s="5">
-        <v>2</v>
-      </c>
-      <c r="J6" s="5">
-        <v>1</v>
-      </c>
-      <c r="K6" s="5">
+      <c r="M6" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" s="5">
         <v>12</v>
@@ -1208,30 +1317,36 @@
         <v>1.5</v>
       </c>
       <c r="E7" s="5">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F7" s="5">
+        <v>30</v>
+      </c>
+      <c r="G7" s="5">
         <v>1200</v>
       </c>
-      <c r="G7" s="5">
-        <v>1</v>
-      </c>
       <c r="H7" s="5">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="I7" s="5">
         <v>2</v>
       </c>
       <c r="J7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="5">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5">
         <v>1</v>
       </c>
-      <c r="K7" s="5">
+      <c r="M7" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" s="5">
         <v>12</v>
@@ -1246,25 +1361,31 @@
         <v>3</v>
       </c>
       <c r="F8" s="5">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5">
         <v>1200</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="5">
         <v>2</v>
       </c>
-      <c r="H8" s="5">
-        <v>3</v>
-      </c>
       <c r="I8" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="5">
         <v>2</v>
       </c>
-      <c r="J8" s="5">
+      <c r="L8" s="5">
         <v>1</v>
       </c>
-      <c r="K8" s="5">
+      <c r="M8" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1278,11 +1399,12 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:K1"/>
+  <mergeCells count="1">
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data reference from table
</commit_message>
<xml_diff>
--- a/TableBuilder/xlsx_Data/PropertyTable.xlsx
+++ b/TableBuilder/xlsx_Data/PropertyTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="132">
   <si>
     <t>!EndOfTable</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -389,10 +389,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Human common</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>All Common</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -410,62 +406,6 @@
   </si>
   <si>
     <t>Player</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>wander_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>min_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>range</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>wander_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>max_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>range</t>
-    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -500,12 +440,85 @@
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Human common</t>
+  </si>
+  <si>
+    <t>normal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchRange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chaseRange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>awayRange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>!Float</t>
+  </si>
+  <si>
+    <r>
+      <t>wander_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>min_range</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ttackRange</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>wander_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>max_range</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,8 +598,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,6 +651,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -693,7 +720,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -725,8 +752,11 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -764,22 +794,29 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="10" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="10" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="10" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="9" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="40% - Accent1" xfId="9" builtinId="31"/>
     <cellStyle name="40% - Accent4" xfId="10" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="7" builtinId="47"/>
+    <cellStyle name="40% - Accent6" xfId="11" builtinId="51"/>
     <cellStyle name="Good" xfId="8" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1089,119 +1126,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.19921875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.3984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.19921875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="M1" s="13"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="Q1" s="15"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="K2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="K2" s="12" t="s">
+      <c r="N2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>104</v>
+      <c r="F3" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>104</v>
@@ -1212,19 +1269,31 @@
       <c r="K3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="R3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1238,8 +1307,12 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>115</v>
       </c>
@@ -1252,140 +1325,180 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="5">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5">
         <v>100</v>
       </c>
-      <c r="L5" s="5">
+      <c r="P5" s="5">
         <v>1</v>
       </c>
-      <c r="M5" s="5">
+      <c r="Q5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="5">
         <v>15</v>
       </c>
       <c r="C6" s="5">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5">
+        <v>15</v>
+      </c>
+      <c r="E6" s="5">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5">
+        <v>20</v>
+      </c>
+      <c r="G6" s="5">
+        <v>20</v>
+      </c>
+      <c r="H6" s="5">
+        <v>30</v>
+      </c>
+      <c r="I6" s="5">
         <v>5</v>
       </c>
-      <c r="D6" s="5">
+      <c r="J6" s="5">
         <v>1.5</v>
       </c>
-      <c r="E6" s="5">
-        <v>15</v>
-      </c>
-      <c r="F6" s="5">
-        <v>30</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="K6" s="5">
         <v>1200</v>
       </c>
-      <c r="H6" s="5">
+      <c r="L6" s="5">
         <v>1.4</v>
       </c>
-      <c r="I6" s="5">
+      <c r="M6" s="5">
         <v>2.1</v>
       </c>
-      <c r="J6" s="5">
+      <c r="N6" s="5">
         <v>0.5</v>
       </c>
-      <c r="K6" s="5">
+      <c r="O6" s="5">
         <v>2</v>
       </c>
-      <c r="L6" s="5">
+      <c r="P6" s="5">
         <v>1</v>
       </c>
-      <c r="M6" s="5">
+      <c r="Q6" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="5">
         <v>12</v>
       </c>
       <c r="C7" s="5">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5">
+        <v>15</v>
+      </c>
+      <c r="E7" s="5">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5">
+        <v>20</v>
+      </c>
+      <c r="G7" s="5">
+        <v>20</v>
+      </c>
+      <c r="H7" s="5">
+        <v>30</v>
+      </c>
+      <c r="I7" s="5">
         <v>5</v>
       </c>
-      <c r="D7" s="5">
+      <c r="J7" s="5">
         <v>1.5</v>
       </c>
-      <c r="E7" s="5">
-        <v>15</v>
-      </c>
-      <c r="F7" s="5">
-        <v>30</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="K7" s="5">
         <v>1200</v>
       </c>
-      <c r="H7" s="5">
+      <c r="L7" s="5">
         <v>1.2</v>
       </c>
-      <c r="I7" s="5">
+      <c r="M7" s="5">
         <v>2</v>
       </c>
-      <c r="J7" s="5">
+      <c r="N7" s="5">
         <v>0.5</v>
       </c>
-      <c r="K7" s="5">
+      <c r="O7" s="5">
         <v>2</v>
       </c>
-      <c r="L7" s="5">
+      <c r="P7" s="5">
         <v>1</v>
       </c>
-      <c r="M7" s="5">
+      <c r="Q7" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="5">
         <v>12</v>
       </c>
       <c r="C8" s="5">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5">
+        <v>20</v>
+      </c>
+      <c r="G8" s="5">
+        <v>20</v>
+      </c>
+      <c r="H8" s="5">
+        <v>30</v>
+      </c>
+      <c r="I8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="5">
+      <c r="J8" s="5">
         <v>1.5</v>
       </c>
-      <c r="E8" s="5">
-        <v>3</v>
-      </c>
-      <c r="F8" s="5">
-        <v>4</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="K8" s="5">
         <v>1200</v>
       </c>
-      <c r="H8" s="5">
+      <c r="L8" s="5">
         <v>2</v>
       </c>
-      <c r="I8" s="5">
+      <c r="M8" s="5">
         <v>3.5</v>
       </c>
-      <c r="J8" s="5">
+      <c r="N8" s="5">
         <v>0.5</v>
       </c>
-      <c r="K8" s="5">
+      <c r="O8" s="5">
         <v>2</v>
       </c>
-      <c r="L8" s="5">
+      <c r="P8" s="5">
         <v>1</v>
       </c>
-      <c r="M8" s="5">
+      <c r="Q8" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1401,10 +1514,14 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Polish AI Chase & Attack
</commit_message>
<xml_diff>
--- a/TableBuilder/xlsx_Data/PropertyTable.xlsx
+++ b/TableBuilder/xlsx_Data/PropertyTable.xlsx
@@ -373,10 +373,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>life</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>format</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -511,6 +507,10 @@
       </rPr>
       <t>max_range</t>
     </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_life</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -756,7 +756,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -800,15 +800,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="10" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="9" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="9" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="9" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1128,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1148,7 +1151,7 @@
     <col min="14" max="14" width="11.19921875" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31.19921875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1156,17 +1159,17 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J1" s="13"/>
       <c r="K1" s="13"/>
@@ -1174,35 +1177,35 @@
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
-      <c r="P1" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q1" s="15"/>
+      <c r="P1" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>127</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>106</v>
@@ -1211,7 +1214,7 @@
         <v>107</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>108</v>
@@ -1220,7 +1223,7 @@
         <v>109</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>110</v>
@@ -1229,7 +1232,7 @@
         <v>111</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>1</v>
@@ -1237,28 +1240,28 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="C3" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>128</v>
+      <c r="F3" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>104</v>
@@ -1288,12 +1291,12 @@
         <v>104</v>
       </c>
       <c r="R3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1314,7 +1317,7 @@
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1341,7 +1344,7 @@
     </row>
     <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="5">
         <v>15</v>
@@ -1380,7 +1383,7 @@
         <v>2.1</v>
       </c>
       <c r="N6" s="5">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="O6" s="5">
         <v>2</v>
@@ -1394,7 +1397,7 @@
     </row>
     <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="5">
         <v>12</v>
@@ -1433,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="N7" s="5">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="O7" s="5">
         <v>2</v>
@@ -1447,7 +1450,7 @@
     </row>
     <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="5">
         <v>12</v>
@@ -1486,7 +1489,7 @@
         <v>3.5</v>
       </c>
       <c r="N8" s="5">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="O8" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
Modify Runaway condition and regenerated health
</commit_message>
<xml_diff>
--- a/TableBuilder/xlsx_Data/PropertyTable.xlsx
+++ b/TableBuilder/xlsx_Data/PropertyTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="133">
   <si>
     <t>!EndOfTable</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -511,6 +511,34 @@
   </si>
   <si>
     <t>max_life</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>print</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Speed</t>
+    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -808,11 +836,11 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="9" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="9" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="9" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1129,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1147,15 +1175,15 @@
     <col min="10" max="10" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.09765625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.19921875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.19921875" customWidth="1"/>
+    <col min="13" max="14" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.19921875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1177,16 +1205,17 @@
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
-      <c r="P1" s="17" t="s">
+      <c r="P1" s="13"/>
+      <c r="Q1" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="17"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="R1" s="18"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>105</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -1198,7 +1227,7 @@
       <c r="E2" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>124</v>
       </c>
       <c r="G2" s="16" t="s">
@@ -1223,22 +1252,25 @@
         <v>109</v>
       </c>
       <c r="N2" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="O2" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>113</v>
       </c>
@@ -1284,17 +1316,20 @@
       <c r="O3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="12" t="s">
         <v>104</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="S3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>118</v>
       </c>
@@ -1314,8 +1349,9 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
-    </row>
-    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R4" s="5"/>
+    </row>
+    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>114</v>
       </c>
@@ -1332,17 +1368,18 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5">
         <v>100</v>
-      </c>
-      <c r="P5" s="5">
-        <v>1</v>
       </c>
       <c r="Q5" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>117</v>
       </c>
@@ -1383,19 +1420,22 @@
         <v>2.1</v>
       </c>
       <c r="N6" s="5">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="O6" s="5">
         <v>1.2</v>
       </c>
-      <c r="O6" s="5">
-        <v>2</v>
-      </c>
       <c r="P6" s="5">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="5">
         <v>1</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="R6" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>116</v>
       </c>
@@ -1436,19 +1476,22 @@
         <v>2</v>
       </c>
       <c r="N7" s="5">
+        <v>4</v>
+      </c>
+      <c r="O7" s="5">
         <v>1.2</v>
       </c>
-      <c r="O7" s="5">
-        <v>2</v>
-      </c>
       <c r="P7" s="5">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="5">
         <v>1</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="R7" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>119</v>
       </c>
@@ -1489,19 +1532,22 @@
         <v>3.5</v>
       </c>
       <c r="N8" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="O8" s="5">
         <v>1.2</v>
       </c>
-      <c r="O8" s="5">
-        <v>2</v>
-      </c>
       <c r="P8" s="5">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="5">
         <v>1</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="R8" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1521,10 +1567,11 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implement UI menus & functions
</commit_message>
<xml_diff>
--- a/TableBuilder/xlsx_Data/PropertyTable.xlsx
+++ b/TableBuilder/xlsx_Data/PropertyTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="134">
   <si>
     <t>!EndOfTable</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -510,10 +510,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>max_life</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>s</t>
     </r>
@@ -539,6 +535,14 @@
       </rPr>
       <t>Speed</t>
     </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>attack_interval</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_health</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1157,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1179,11 +1183,12 @@
     <col min="15" max="15" width="11.19921875" style="1" customWidth="1"/>
     <col min="16" max="16" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.19921875" customWidth="1"/>
+    <col min="18" max="18" width="12.296875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1210,8 +1215,9 @@
         <v>115</v>
       </c>
       <c r="R1" s="18"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="S1" s="18"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>109</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O2" s="14" t="s">
         <v>120</v>
@@ -1264,13 +1270,16 @@
         <v>111</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="S2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>113</v>
       </c>
@@ -1325,11 +1334,14 @@
       <c r="R3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="T3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>118</v>
       </c>
@@ -1350,8 +1362,9 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
-    </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>114</v>
       </c>
@@ -1373,13 +1386,14 @@
         <v>100</v>
       </c>
       <c r="Q5" s="5">
+        <v>5</v>
+      </c>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5">
         <v>1</v>
       </c>
-      <c r="R5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>117</v>
       </c>
@@ -1429,13 +1443,16 @@
         <v>8</v>
       </c>
       <c r="Q6" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R6" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>0.3</v>
+      </c>
+      <c r="S6" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>116</v>
       </c>
@@ -1485,13 +1502,16 @@
         <v>8</v>
       </c>
       <c r="Q7" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R7" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>0.3</v>
+      </c>
+      <c r="S7" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>119</v>
       </c>
@@ -1541,13 +1561,16 @@
         <v>8</v>
       </c>
       <c r="Q8" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R8" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>0.3</v>
+      </c>
+      <c r="S8" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1568,10 +1591,11 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Attach Sounds and Menus
</commit_message>
<xml_diff>
--- a/TableBuilder/xlsx_Data/PropertyTable.xlsx
+++ b/TableBuilder/xlsx_Data/PropertyTable.xlsx
@@ -1163,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1386,7 +1386,7 @@
         <v>100</v>
       </c>
       <c r="Q5" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R5" s="5"/>
       <c r="S5" s="5">
@@ -1443,10 +1443,10 @@
         <v>8</v>
       </c>
       <c r="Q6" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R6" s="5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="S6" s="5">
         <v>50</v>
@@ -1502,10 +1502,10 @@
         <v>8</v>
       </c>
       <c r="Q7" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R7" s="5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="S7" s="5">
         <v>50</v>
@@ -1564,10 +1564,10 @@
         <v>5</v>
       </c>
       <c r="R8" s="5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="S8" s="5">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
bug fix - sound pool and AI
</commit_message>
<xml_diff>
--- a/TableBuilder/xlsx_Data/PropertyTable.xlsx
+++ b/TableBuilder/xlsx_Data/PropertyTable.xlsx
@@ -1164,7 +1164,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1386,7 +1386,7 @@
         <v>100</v>
       </c>
       <c r="Q5" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R5" s="5"/>
       <c r="S5" s="5">
@@ -1443,7 +1443,7 @@
         <v>8</v>
       </c>
       <c r="Q6" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6" s="5">
         <v>0.4</v>
@@ -1502,7 +1502,7 @@
         <v>8</v>
       </c>
       <c r="Q7" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" s="5">
         <v>0.4</v>
@@ -1567,7 +1567,7 @@
         <v>0.4</v>
       </c>
       <c r="S8" s="5">
-        <v>1000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>